<commit_message>
faire du excel cestrigolo
</commit_message>
<xml_diff>
--- a/Excel/Staigiare AFPA.xlsx
+++ b/Excel/Staigiare AFPA.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="114">
   <si>
     <t>adresse</t>
   </si>
@@ -371,6 +371,12 @@
   </si>
   <si>
     <t>Insertion SQL</t>
+  </si>
+  <si>
+    <t>idHebergement</t>
+  </si>
+  <si>
+    <t>libelleHebergement</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1329,7 @@
     <col min="2" max="2" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" style="6" bestFit="1" customWidth="1"/>
@@ -2146,16 +2152,39 @@
       <c r="A35" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="D35" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N35" s="13" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>85</v>
       </c>
+      <c r="D36" s="11">
+        <v>1</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N36" s="13"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>86</v>
       </c>
+      <c r="D37" s="13">
+        <v>2</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N37" s="13"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>